<commit_message>
Added functionality to set test data from excel
</commit_message>
<xml_diff>
--- a/Module20/TestAutomation/TestData/Suite.xlsx
+++ b/Module20/TestAutomation/TestData/Suite.xlsx
@@ -387,7 +387,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -398,7 +398,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>